<commit_message>
fixed the sound sheet of the guide
</commit_message>
<xml_diff>
--- a/concept/sound/the_guide_sounds_sheet.xlsx
+++ b/concept/sound/the_guide_sounds_sheet.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="69">
   <si>
     <t>Start</t>
   </si>
@@ -168,12 +168,6 @@
     <t>Third Encounter Pre Demon Huntress: Wenn ihn Scarlet das erste Mal an diesem Ort anspricht und die Twin Fairies besiegt hat (aufnahme leider in 2 takes)</t>
   </si>
   <si>
-    <t>01:28.6 &amp; 01:34.4</t>
-  </si>
-  <si>
-    <t>01:33.2 &amp; 01:39.0</t>
-  </si>
-  <si>
     <t>01:39.3</t>
   </si>
   <si>
@@ -184,9 +178,6 @@
   </si>
   <si>
     <t>01:46.5</t>
-  </si>
-  <si>
-    <t>01:52.9</t>
   </si>
   <si>
     <r>
@@ -254,49 +245,31 @@
     <t>Third Encounter Pre Demon Huntress: Wenn ihn Scarlet das dritte Mal an diesem Ort anspricht</t>
   </si>
   <si>
-    <t>02:14.6</t>
-  </si>
-  <si>
-    <t>02:20.3</t>
-  </si>
-  <si>
-    <t>Third Encounter Pre Demon Huntress: Wenn ihn Scarlet das vierte Mal an diesem Ort anspricht</t>
-  </si>
-  <si>
-    <t>02:21.1</t>
-  </si>
-  <si>
-    <t>02:28.9</t>
-  </si>
-  <si>
-    <t>Third Encounter Pre Demon Huntress: Wenn ihn Scarlet das fünfte Mal an diesem Ort anspricht</t>
-  </si>
-  <si>
-    <t>02:30.04</t>
-  </si>
-  <si>
-    <t>02:40.2</t>
-  </si>
-  <si>
-    <t>Third Encounter Pre Demon Huntress: Wenn ihn Scarlet das sechste Mal an diesem Ort anspricht</t>
-  </si>
-  <si>
-    <t>02:40.4</t>
-  </si>
-  <si>
-    <t>02:49.0</t>
-  </si>
-  <si>
     <t>Third Encounter Pre Demon Huntress: Wenn ihn Scarlet das siebte Mal an diesem Ort anspricht (dieser Wiederholt sich an diesem Ort bei jedem weiteren Mal ansprechen)</t>
   </si>
   <si>
-    <t>02:50.7</t>
-  </si>
-  <si>
     <t>02:58.1</t>
   </si>
   <si>
     <t>Credits Cutscene / Post Angel / True Ending: Wenn Scarlet auf die Erde blickt und diese in ihrer Aura eingeschlossen wird</t>
+  </si>
+  <si>
+    <t>01:27.5</t>
+  </si>
+  <si>
+    <t>01:36.4</t>
+  </si>
+  <si>
+    <t>01:51.9</t>
+  </si>
+  <si>
+    <t>02:45.4</t>
+  </si>
+  <si>
+    <t>02:53.8</t>
+  </si>
+  <si>
+    <t>03:05.5</t>
   </si>
 </sst>
 </file>
@@ -360,7 +333,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="61">
+  <cellStyleXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -422,17 +395,20 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="61">
+  <cellStyles count="65">
     <cellStyle name="Besuchter Link" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="6" builtinId="9" hidden="1"/>
@@ -463,6 +439,8 @@
     <cellStyle name="Besuchter Link" xfId="56" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="58" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="64" builtinId="9" hidden="1"/>
     <cellStyle name="Link" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="5" builtinId="8" hidden="1"/>
@@ -493,6 +471,8 @@
     <cellStyle name="Link" xfId="55" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="57" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="63" builtinId="8" hidden="1"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -825,7 +805,7 @@
   <dimension ref="A1:F35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1091,12 +1071,12 @@
         <v>47</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="30">
+    <row r="16" spans="1:6">
       <c r="A16" s="3" t="s">
-        <v>49</v>
+        <v>63</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>50</v>
+        <v>64</v>
       </c>
       <c r="C16" t="s">
         <v>5</v>
@@ -1110,10 +1090,10 @@
     </row>
     <row r="17" spans="1:5">
       <c r="A17" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B17" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C17" t="s">
         <v>5</v>
@@ -1122,15 +1102,15 @@
         <v>7</v>
       </c>
       <c r="E17" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B18" t="s">
-        <v>55</v>
+        <v>65</v>
       </c>
       <c r="C18" t="s">
         <v>5</v>
@@ -1139,15 +1119,15 @@
         <v>7</v>
       </c>
       <c r="E18" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B19" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C19" t="s">
         <v>5</v>
@@ -1156,15 +1136,15 @@
         <v>7</v>
       </c>
       <c r="E19" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B20" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C20" t="s">
         <v>5</v>
@@ -1173,15 +1153,15 @@
         <v>7</v>
       </c>
       <c r="E20" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="B21" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="C21" t="s">
         <v>5</v>
@@ -1190,84 +1170,33 @@
         <v>7</v>
       </c>
       <c r="E21" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
     </row>
     <row r="22" spans="1:5">
       <c r="A22" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="B22" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C22" t="s">
         <v>5</v>
       </c>
       <c r="D22" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E22" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5">
-      <c r="A23" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="B23" t="s">
-        <v>70</v>
-      </c>
-      <c r="C23" t="s">
-        <v>5</v>
-      </c>
-      <c r="D23" t="s">
-        <v>7</v>
-      </c>
-      <c r="E23" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
     </row>
     <row r="24" spans="1:5">
-      <c r="A24" t="s">
-        <v>72</v>
-      </c>
-      <c r="B24" t="s">
-        <v>73</v>
-      </c>
-      <c r="C24" t="s">
-        <v>5</v>
-      </c>
-      <c r="D24" t="s">
-        <v>7</v>
-      </c>
-      <c r="E24" t="s">
-        <v>74</v>
-      </c>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
     </row>
     <row r="25" spans="1:5">
-      <c r="A25" t="s">
-        <v>75</v>
-      </c>
-      <c r="B25" t="s">
-        <v>76</v>
-      </c>
-      <c r="C25" t="s">
-        <v>5</v>
-      </c>
-      <c r="D25" t="s">
-        <v>6</v>
-      </c>
-      <c r="E25" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5">
-      <c r="C27" s="1"/>
-      <c r="D27" s="1"/>
-    </row>
-    <row r="28" spans="1:5">
-      <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
     </row>
     <row r="29" spans="1:5">
       <c r="C29" s="1"/>

</xml_diff>